<commit_message>
alteração de restrição - terceirizada
</commit_message>
<xml_diff>
--- a/IdUnico - enviado para o professor/solicitacaoMudanca.xlsx
+++ b/IdUnico - enviado para o professor/solicitacaoMudanca.xlsx
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="43">
   <si>
     <t>IdUnico - SOLICITAÇÃO DE MUDANÇA - Gestão de Projeto de Software II (2015.1)</t>
   </si>
@@ -273,6 +273,12 @@
   </si>
   <si>
     <t>Foi incluído na EAP atividade de gerenciamento de equipes</t>
+  </si>
+  <si>
+    <t>Não estava explicito no escopo que a produção do chip e leitor seriam feito de forma terceirizada. </t>
+  </si>
+  <si>
+    <t>Foi incluído uma restrição da declaração de escopo.</t>
   </si>
 </sst>
 </file>
@@ -426,8 +432,8 @@
   </sheetPr>
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -647,7 +653,7 @@
       </c>
       <c r="F11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="37.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="43.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>9</v>
       </c>
@@ -665,24 +671,42 @@
       </c>
       <c r="F12" s="7"/>
     </row>
-    <row r="13" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" customFormat="false" ht="35.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="D13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>

</xml_diff>